<commit_message>
Fixed spreadsheet for Lab02
</commit_message>
<xml_diff>
--- a/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="111">
   <si>
     <t xml:space="preserve">VVSS, Info Romana, 2024-2025</t>
   </si>
@@ -133,27 +133,7 @@
     <t xml:space="preserve">Un cinefil doreşte să îşi dezvolte un program pentru gestionarea filmelor din colecţia personală. Programul va permite următoarele operaţii:</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">F01.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> adăugarea unui film nou (titlu, regizor, an aparitie, actori, categorie, cuvinte cheie);</t>
-    </r>
+    <t xml:space="preserve">F01. Adaugarea unui task nou cu detaliile: descrierea, data si ora de inceput, data si ora de sfarsit. Daca task-ul este repetitiv, atunci se indica intervalul de timp la care se va repeta, dat ca numar de ore si minute. Task-ul poate fi activ sau nu.</t>
   </si>
   <si>
     <t xml:space="preserve">Observații</t>
@@ -162,7 +142,7 @@
     <t xml:space="preserve">1. La proiectarea TCs se consideră o metodă care poate avea următoarea semnătură: </t>
   </si>
   <si>
-    <t xml:space="preserve">addMovie(String title, String director, int year, List&lt;String&gt; actors, String category, List&lt;String&gt; keywords): void</t>
+    <t xml:space="preserve">Void addTask(Task task)</t>
   </si>
   <si>
     <t xml:space="preserve">2. Metoda este definită la nivelul repository, service sau ui.</t>
@@ -309,66 +289,66 @@
     <t xml:space="preserve">output data</t>
   </si>
   <si>
-    <t xml:space="preserve">title.lentgh&gt;0</t>
+    <t xml:space="preserve">title not null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">startTIme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,3</t>
   </si>
   <si>
     <t xml:space="preserve">meeting</t>
   </si>
   <si>
-    <t xml:space="preserve">title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">startTIme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">endTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interval</t>
-  </si>
-  <si>
-    <t xml:space="preserve">active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expected</t>
+    <t xml:space="preserve">2025.04.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025.04.06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">task added succesfully</t>
+  </si>
+  <si>
+    <t xml:space="preserve">startTime not null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,3</t>
   </si>
   <si>
     <t xml:space="preserve">null</t>
   </si>
   <si>
-    <t xml:space="preserve">1,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025.04.05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025.04.06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">task added succesfully</t>
-  </si>
-  <si>
-    <t xml:space="preserve">startTime not null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025.04.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,3</t>
-  </si>
-  <si>
     <t xml:space="preserve">error throws invalid argument exception</t>
   </si>
   <si>
+    <t xml:space="preserve">startTime null</t>
+  </si>
+  <si>
     <t xml:space="preserve">1,4</t>
   </si>
   <si>
     <t xml:space="preserve">meeting1</t>
   </si>
   <si>
-    <t xml:space="preserve">2,4</t>
-  </si>
-  <si>
     <t xml:space="preserve">…</t>
   </si>
   <si>
@@ -411,7 +391,7 @@
     <t xml:space="preserve">title.length=1</t>
   </si>
   <si>
-    <t xml:space="preserve">TC3_EC</t>
+    <t xml:space="preserve">TC5_BVA</t>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
@@ -423,52 +403,52 @@
     <t xml:space="preserve">Hello world</t>
   </si>
   <si>
+    <t xml:space="preserve">StartTime &lt;= endTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StartTime = endTIme + 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StartTime = endTIme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StartTime = endTime – 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BBT TCs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final        TC No.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req. ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECP TCs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BVA TCs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actual result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC1_ECP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
     <t xml:space="preserve">Meeting</t>
   </si>
   <si>
-    <t xml:space="preserve">StartTime &lt;= endTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StartTime &gt; endTIme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StartTime = endTIme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StartTime &lt; endTime </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BBT TCs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Final        TC No.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Req. ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECP TCs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BVA TCs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">actual result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC1_ECP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
     <t xml:space="preserve">2,3,2</t>
   </si>
   <si>
-    <t xml:space="preserve">No exception thrown</t>
+    <t xml:space="preserve">Task added successfully</t>
   </si>
   <si>
     <t xml:space="preserve">TC2_ECP</t>
@@ -589,7 +569,7 @@
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -738,6 +718,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -988,404 +975,412 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="102">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="7" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="7" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="7" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="7" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1645,217 +1640,217 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="32.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="32.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="20"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="H1" s="2" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="4" t="n">
+      <c r="J4" s="5" t="n">
         <v>235</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="4" t="n">
+      <c r="J5" s="5" t="n">
         <v>235</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="5"/>
-      <c r="H6" s="4" t="s">
+      <c r="B6" s="6"/>
+      <c r="H6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="4" t="n">
+      <c r="J6" s="5" t="n">
         <v>235</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11" t="s">
+      <c r="A24" s="11"/>
+      <c r="B24" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="12"/>
+      <c r="C26" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1887,429 +1882,418 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="29.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="25.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="29.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="G5" s="15" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="G5" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16" t="s">
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="16"/>
+      <c r="O6" s="17"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="18" t="n">
+      <c r="B7" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16" t="s">
+      <c r="J7" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="K7" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="L7" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="16" t="s">
+      <c r="M7" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="N7" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="O7" s="17"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="O7" s="16"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="18" t="n">
+      <c r="G8" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="M8" s="21" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="19" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="G9" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="16" t="n">
+      <c r="H9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="M9" s="21" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" s="4" t="s">
+      <c r="N9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="19" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="L8" s="4" t="n">
+      <c r="L10" s="23" t="n">
         <v>30</v>
       </c>
-      <c r="M8" s="20" t="b">
+      <c r="M10" s="24" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="N8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="18" t="n">
-        <v>3</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="18"/>
-      <c r="G9" s="16" t="n">
-        <v>2</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L9" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="M9" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="N9" s="3" t="s">
+      <c r="N10" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="O9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="18" t="n">
+      <c r="O10" s="25"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="19" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="G11" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="H10" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="I10" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="J10" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="K10" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" s="22" t="n">
-        <v>30</v>
-      </c>
-      <c r="M10" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="N10" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="O10" s="24"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="18" t="n">
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="19" t="n">
+        <v>6</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="G12" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="G11" s="21" t="n">
-        <v>4</v>
-      </c>
-      <c r="H11" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="K11" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="L11" s="22" t="n">
-        <v>30</v>
-      </c>
-      <c r="M11" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="N11" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="O11" s="24"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="18" t="n">
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="19" t="n">
+        <v>7</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="G13" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="G12" s="25" t="n">
-        <v>5</v>
-      </c>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="18" t="n">
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="19" t="n">
+        <v>8</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="G14" s="29" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="G13" s="25" t="n">
-        <v>6</v>
-      </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="18" t="n">
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="19" t="n">
+        <v>9</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="G15" s="29" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="G14" s="28" t="n">
-        <v>7</v>
-      </c>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="18" t="n">
-        <v>9</v>
-      </c>
-      <c r="C15" s="19" t="s">
+      <c r="H15" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="G15" s="28" t="n">
-        <v>8</v>
-      </c>
-      <c r="H15" s="29" t="s">
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="19" t="n">
+        <v>10</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="19" t="n">
+        <v>11</v>
+      </c>
+      <c r="C17" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="18" t="n">
-        <v>10</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="18" t="n">
-        <v>11</v>
-      </c>
-      <c r="C17" s="19" t="s">
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="19" t="n">
+        <v>12</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="19" t="n">
+        <v>13</v>
+      </c>
+      <c r="C19" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="18" t="n">
-        <v>12</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="18" t="n">
-        <v>13</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="30"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="18" t="n">
+      <c r="B20" s="19" t="n">
         <v>14</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="29">
@@ -2362,615 +2346,612 @@
   <dimension ref="B1:Q30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M9" activeCellId="0" sqref="M9"/>
+      <selection pane="topLeft" activeCell="P11" activeCellId="0" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="23.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="21.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="23.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="33"/>
-      <c r="G5" s="15" t="s">
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="34"/>
+      <c r="G5" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="G6" s="17" t="s">
+      <c r="E6" s="35"/>
+      <c r="G6" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="J6" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="35" t="s">
+      <c r="K6" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35" t="s">
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="35"/>
+      <c r="Q6" s="36"/>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="18" t="n">
+      <c r="B7" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="L7" s="16" t="s">
+      <c r="E7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="M7" s="17" t="s">
+      <c r="M7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="17" t="s">
+      <c r="O7" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="O7" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="P7" s="16" t="s">
+      <c r="P7" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="Q7" s="16"/>
+      <c r="Q7" s="17"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="18"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="4" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="16" t="n">
+      <c r="E8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="H8" s="37" t="n">
+      <c r="H8" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="38" t="s">
+      <c r="I8" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="38" t="s">
+      <c r="J8" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="K8" s="39"/>
-      <c r="L8" s="40" t="n">
+      <c r="K8" s="40"/>
+      <c r="L8" s="41" t="n">
         <v>45752</v>
       </c>
-      <c r="M8" s="40" t="n">
+      <c r="M8" s="41" t="n">
         <v>45753</v>
       </c>
-      <c r="N8" s="39" t="n">
+      <c r="N8" s="40" t="n">
         <v>30</v>
       </c>
-      <c r="O8" s="41" t="b">
+      <c r="O8" s="42" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="P8" s="24" t="s">
+      <c r="P8" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="Q8" s="24"/>
+      <c r="Q8" s="25"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="18"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="4"/>
-      <c r="G9" s="28" t="n">
+      <c r="B9" s="19"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="5"/>
+      <c r="G9" s="29" t="n">
         <v>2</v>
       </c>
-      <c r="H9" s="42" t="n">
+      <c r="H9" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="I9" s="38" t="s">
+      <c r="I9" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="K9" s="43" t="s">
+      <c r="K9" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="L9" s="40" t="n">
+      <c r="L9" s="41" t="n">
         <v>45752</v>
       </c>
-      <c r="M9" s="40" t="n">
+      <c r="M9" s="41" t="n">
         <v>45753</v>
       </c>
-      <c r="N9" s="39" t="n">
+      <c r="N9" s="40" t="n">
         <v>30</v>
       </c>
-      <c r="O9" s="41" t="b">
+      <c r="O9" s="42" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="P9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="Q9" s="3"/>
+      <c r="Q9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="18"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="4"/>
-      <c r="G10" s="16" t="n">
+      <c r="B10" s="19"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="5"/>
+      <c r="G10" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="H10" s="37" t="n">
+      <c r="H10" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="I10" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="J10" s="38" t="s">
+      <c r="I10" s="39"/>
+      <c r="J10" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="K10" s="44" t="s">
+      <c r="K10" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="L10" s="40" t="n">
+      <c r="L10" s="41" t="n">
         <v>45756</v>
       </c>
-      <c r="M10" s="40" t="n">
+      <c r="M10" s="41" t="n">
+        <v>45755</v>
+      </c>
+      <c r="N10" s="40" t="n">
+        <v>30</v>
+      </c>
+      <c r="O10" s="42" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="P10" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q10" s="25"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="19"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="5"/>
+      <c r="G11" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="H11" s="38" t="n">
+        <v>4</v>
+      </c>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="41" t="n">
         <v>45753</v>
       </c>
-      <c r="N10" s="39" t="n">
+      <c r="M11" s="41" t="n">
+        <v>45753</v>
+      </c>
+      <c r="N11" s="40" t="n">
         <v>30</v>
       </c>
-      <c r="O10" s="41" t="b">
+      <c r="O11" s="42" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="P10" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q10" s="24"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="18"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="4"/>
-      <c r="G11" s="16" t="n">
+      <c r="P11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="19"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="5"/>
+      <c r="G12" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H12" s="38"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="19" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" s="29" t="n">
+        <v>6</v>
+      </c>
+      <c r="H13" s="43"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="H11" s="37" t="n">
+      <c r="G14" s="17" t="n">
+        <v>7</v>
+      </c>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="39"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G15" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="H15" s="38"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="5"/>
+      <c r="G16" s="17" t="n">
+        <v>9</v>
+      </c>
+      <c r="H16" s="38"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="5"/>
+      <c r="G17" s="17" t="n">
+        <v>10</v>
+      </c>
+      <c r="H17" s="38"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="39"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="5"/>
+      <c r="G18" s="17" t="n">
+        <v>11</v>
+      </c>
+      <c r="H18" s="38"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="39"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="19" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" s="37"/>
+      <c r="D19" s="5"/>
+      <c r="G19" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="H19" s="38"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="39"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="19"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="5"/>
+      <c r="G20" s="17" t="n">
+        <v>13</v>
+      </c>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="39"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="19"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="5"/>
+      <c r="G21" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="H21" s="38"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="39"/>
+      <c r="Q21" s="39"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="19"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="5"/>
+      <c r="G22" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="H22" s="38"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="39"/>
+      <c r="Q22" s="39"/>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="19"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="5"/>
+      <c r="G23" s="17" t="n">
+        <v>16</v>
+      </c>
+      <c r="H23" s="38"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="39"/>
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="19"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="5"/>
+      <c r="G24" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H24" s="38"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="40"/>
+      <c r="P24" s="39"/>
+      <c r="Q24" s="39"/>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="I11" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="J11" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="K11" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="L11" s="40" t="n">
-        <v>45753</v>
-      </c>
-      <c r="M11" s="40" t="n">
-        <v>45753</v>
-      </c>
-      <c r="N11" s="39" t="n">
-        <v>30</v>
-      </c>
-      <c r="O11" s="41" t="b">
-        <v>1</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="18"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="4"/>
-      <c r="G12" s="16" t="n">
-        <v>5</v>
-      </c>
-      <c r="H12" s="37" t="n">
-        <v>5</v>
-      </c>
-      <c r="I12" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="J12" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="K12" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="L12" s="40" t="n">
-        <v>45757</v>
-      </c>
-      <c r="M12" s="40" t="n">
-        <v>45758</v>
-      </c>
-      <c r="N12" s="39" t="n">
-        <v>30</v>
-      </c>
-      <c r="O12" s="41" t="b">
-        <v>0</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" s="28" t="n">
-        <v>6</v>
-      </c>
-      <c r="H13" s="42"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" s="16" t="n">
-        <v>7</v>
-      </c>
-      <c r="H14" s="37"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="38"/>
-      <c r="Q14" s="38"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" s="16" t="n">
-        <v>8</v>
-      </c>
-      <c r="H15" s="37"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="38"/>
-      <c r="Q15" s="38"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="4"/>
-      <c r="G16" s="16" t="n">
-        <v>9</v>
-      </c>
-      <c r="H16" s="37"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="38"/>
-      <c r="Q16" s="38"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="4"/>
-      <c r="G17" s="16" t="n">
-        <v>10</v>
-      </c>
-      <c r="H17" s="37"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="38"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="4"/>
-      <c r="G18" s="16" t="n">
-        <v>11</v>
-      </c>
-      <c r="H18" s="37"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="38"/>
-      <c r="Q18" s="38"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="18" t="n">
-        <v>3</v>
-      </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="4"/>
-      <c r="G19" s="16" t="n">
-        <v>12</v>
-      </c>
-      <c r="H19" s="37"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="39"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="18"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="4"/>
-      <c r="G20" s="16" t="n">
-        <v>13</v>
-      </c>
-      <c r="H20" s="37"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="39"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="18"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="4"/>
-      <c r="G21" s="16" t="n">
-        <v>14</v>
-      </c>
-      <c r="H21" s="37"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="38"/>
-      <c r="Q21" s="38"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="18"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="4"/>
-      <c r="G22" s="16" t="n">
-        <v>15</v>
-      </c>
-      <c r="H22" s="37"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="39"/>
-      <c r="O22" s="39"/>
-      <c r="P22" s="38"/>
-      <c r="Q22" s="38"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="18"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="4"/>
-      <c r="G23" s="16" t="n">
-        <v>16</v>
-      </c>
-      <c r="H23" s="37"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="39"/>
-      <c r="O23" s="39"/>
-      <c r="P23" s="38"/>
-      <c r="Q23" s="38"/>
-    </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="18"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="4"/>
-      <c r="G24" s="16" t="n">
-        <v>17</v>
-      </c>
-      <c r="H24" s="37"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="39"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="18" t="n">
-        <v>4</v>
-      </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="16" t="n">
+      <c r="G25" s="17" t="n">
         <v>18</v>
       </c>
-      <c r="H25" s="37"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="39"/>
-      <c r="O25" s="39"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="39"/>
+      <c r="Q25" s="39"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="18"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="4" t="s">
+      <c r="B26" s="19"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="4" t="s">
+      <c r="B27" s="19"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="18"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="4" t="s">
+      <c r="B28" s="19"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="46"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="47"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="18"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="4" t="s">
+      <c r="B29" s="19"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="48"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="48"/>
+      <c r="M29" s="48"/>
+      <c r="N29" s="49"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="18"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="4" t="s">
+      <c r="B30" s="19"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="5" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3036,558 +3017,566 @@
   <dimension ref="B1:P21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G36" activeCellId="0" sqref="G36"/>
+      <selection pane="topLeft" activeCell="O13" activeCellId="0" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="30.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="30.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="26.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="50" t="s">
+      <c r="C4" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="D4" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="E4" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="F4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" s="17"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="51"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" s="16"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="53" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="N5" s="53" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="56" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="54" t="n">
+      <c r="D6" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="59" t="n">
+        <v>45752</v>
+      </c>
+      <c r="H6" s="59" t="n">
+        <v>45753</v>
+      </c>
+      <c r="I6" s="58" t="n">
+        <v>30</v>
+      </c>
+      <c r="J6" s="60" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C6" s="55" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" s="54" t="s">
-        <v>86</v>
-      </c>
-      <c r="F6" s="57" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" s="58" t="n">
-        <v>45752</v>
-      </c>
-      <c r="H6" s="58" t="n">
-        <v>45753</v>
-      </c>
-      <c r="I6" s="57" t="n">
-        <v>30</v>
-      </c>
-      <c r="J6" s="59" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60" t="s">
+      <c r="K6" s="61"/>
+      <c r="L6" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="M6" s="57" t="s">
+      <c r="M6" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="N6" s="57" t="s">
+      <c r="N6" s="62" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="61" t="n">
+      <c r="B7" s="63" t="n">
         <f aca="false">B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="62" t="s">
+      <c r="C7" s="56"/>
+      <c r="D7" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="61" t="s">
-        <v>86</v>
-      </c>
-      <c r="F7" s="63" t="s">
+      <c r="E7" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="64" t="n">
+      <c r="G7" s="66" t="n">
         <v>45757</v>
       </c>
-      <c r="H7" s="64" t="n">
+      <c r="H7" s="66" t="n">
         <v>45758</v>
       </c>
-      <c r="I7" s="63" t="n">
+      <c r="I7" s="65" t="n">
         <v>30</v>
       </c>
-      <c r="J7" s="65" t="b">
+      <c r="J7" s="67" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="57" t="s">
+      <c r="K7" s="68"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="N7" s="57" t="s">
+      <c r="N7" s="62" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="61" t="n">
+      <c r="B8" s="63" t="n">
         <f aca="false">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="62" t="s">
+      <c r="C8" s="56"/>
+      <c r="D8" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="61" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="68" t="n">
+      <c r="E8" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="70" t="n">
         <v>45752</v>
       </c>
-      <c r="H8" s="68" t="n">
+      <c r="H8" s="70" t="n">
         <v>45753</v>
       </c>
-      <c r="I8" s="67" t="n">
+      <c r="I8" s="69" t="n">
         <v>30</v>
       </c>
-      <c r="J8" s="69" t="b">
+      <c r="J8" s="71" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="61" t="s">
+      <c r="K8" s="69"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="N8" s="61" t="s">
-        <v>91</v>
+      <c r="N8" s="62" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="61" t="n">
+      <c r="B9" s="63" t="n">
         <f aca="false">B8+1</f>
         <v>4</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="62" t="s">
+      <c r="C9" s="56"/>
+      <c r="D9" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="E9" s="61" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" s="61" t="s">
+      <c r="E9" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="G9" s="61" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="70" t="n">
+      <c r="G9" s="63" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="72" t="n">
         <v>45753</v>
       </c>
-      <c r="I9" s="61" t="n">
+      <c r="I9" s="63" t="n">
         <v>30</v>
       </c>
-      <c r="J9" s="71" t="b">
+      <c r="J9" s="73" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="61" t="s">
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="N9" s="61" t="s">
-        <v>91</v>
+      <c r="N9" s="62" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="61" t="n">
+      <c r="B10" s="63" t="n">
         <f aca="false">B9+1</f>
         <v>5</v>
       </c>
-      <c r="C10" s="55"/>
-      <c r="D10" s="62" t="s">
+      <c r="C10" s="56"/>
+      <c r="D10" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="61" t="s">
-        <v>94</v>
-      </c>
-      <c r="F10" s="57" t="s">
-        <v>73</v>
-      </c>
-      <c r="G10" s="58" t="n">
+      <c r="G10" s="59" t="n">
         <v>45752</v>
       </c>
-      <c r="H10" s="58" t="n">
+      <c r="H10" s="59" t="n">
         <v>45753</v>
       </c>
-      <c r="I10" s="57" t="n">
+      <c r="I10" s="58" t="n">
         <v>30</v>
       </c>
-      <c r="J10" s="59" t="b">
+      <c r="J10" s="60" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="57" t="s">
+      <c r="K10" s="75"/>
+      <c r="L10" s="75"/>
+      <c r="M10" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="N10" s="57" t="s">
+      <c r="N10" s="62" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="61" t="n">
+      <c r="B11" s="63" t="n">
         <f aca="false">B10+1</f>
         <v>6</v>
       </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="62" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="61" t="s">
+      <c r="C11" s="56"/>
+      <c r="D11" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="F11" s="63" t="s">
+      <c r="F11" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="G11" s="64" t="n">
+      <c r="G11" s="66" t="n">
         <v>45757</v>
       </c>
-      <c r="H11" s="64" t="n">
+      <c r="H11" s="66" t="n">
         <v>45758</v>
       </c>
-      <c r="I11" s="63" t="n">
+      <c r="I11" s="65" t="n">
         <v>30</v>
       </c>
-      <c r="J11" s="65" t="b">
+      <c r="J11" s="67" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="57" t="s">
+      <c r="K11" s="75"/>
+      <c r="L11" s="75"/>
+      <c r="M11" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="N11" s="57" t="s">
+      <c r="N11" s="62" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="61" t="n">
+      <c r="B12" s="63" t="n">
         <f aca="false">B11+1</f>
         <v>7</v>
       </c>
-      <c r="C12" s="55"/>
-      <c r="D12" s="62" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" s="61" t="s">
+      <c r="C12" s="56"/>
+      <c r="D12" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="63" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="74"/>
-      <c r="G12" s="75" t="n">
+      <c r="F12" s="76"/>
+      <c r="G12" s="77" t="n">
         <v>45752</v>
       </c>
-      <c r="H12" s="75" t="n">
+      <c r="H12" s="77" t="n">
         <v>45753</v>
       </c>
-      <c r="I12" s="76" t="n">
+      <c r="I12" s="78" t="n">
         <v>30</v>
       </c>
-      <c r="J12" s="77" t="b">
+      <c r="J12" s="79" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K12" s="73"/>
-      <c r="L12" s="73"/>
-      <c r="M12" s="61" t="s">
+      <c r="K12" s="75"/>
+      <c r="L12" s="75"/>
+      <c r="M12" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="N12" s="61" t="s">
-        <v>91</v>
+      <c r="N12" s="62" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="78" t="n">
+      <c r="B13" s="80" t="n">
         <f aca="false">B12+1</f>
         <v>8</v>
       </c>
-      <c r="C13" s="55"/>
-      <c r="D13" s="52" t="s">
+      <c r="C13" s="56"/>
+      <c r="D13" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="78" t="s">
+      <c r="E13" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="F13" s="78" t="s">
+      <c r="F13" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="79" t="n">
+      <c r="G13" s="81" t="n">
         <v>45756</v>
       </c>
-      <c r="H13" s="79" t="n">
+      <c r="H13" s="81" t="n">
         <v>45753</v>
       </c>
-      <c r="I13" s="78" t="n">
+      <c r="I13" s="80" t="n">
         <v>30</v>
       </c>
-      <c r="J13" s="80" t="b">
+      <c r="J13" s="82" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="61" t="s">
+      <c r="K13" s="83"/>
+      <c r="L13" s="83"/>
+      <c r="M13" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="N13" s="61" t="s">
-        <v>91</v>
+      <c r="N13" s="62" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="82"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="83"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="82"/>
-      <c r="I14" s="82"/>
-      <c r="J14" s="82"/>
-      <c r="K14" s="82"/>
-      <c r="L14" s="82"/>
-      <c r="M14" s="82"/>
-      <c r="N14" s="82"/>
+      <c r="B14" s="84"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="84"/>
+      <c r="F14" s="84"/>
+      <c r="G14" s="84"/>
+      <c r="H14" s="84"/>
+      <c r="I14" s="84"/>
+      <c r="J14" s="84"/>
+      <c r="K14" s="84"/>
+      <c r="L14" s="84"/>
+      <c r="M14" s="84"/>
+      <c r="N14" s="84"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="84" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="82"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="82"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="85"/>
-      <c r="L15" s="85"/>
-      <c r="M15" s="84"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="86"/>
+      <c r="J15" s="86"/>
+      <c r="K15" s="87"/>
+      <c r="L15" s="87"/>
+      <c r="M15" s="86"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M16" s="84"/>
+      <c r="M16" s="86"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="86" t="s">
+      <c r="C17" s="88" t="s">
         <v>99</v>
       </c>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="87" t="s">
+      <c r="D17" s="88"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="88"/>
+      <c r="G17" s="89" t="s">
         <v>100</v>
       </c>
-      <c r="H17" s="86" t="s">
+      <c r="H17" s="88" t="s">
         <v>101</v>
       </c>
-      <c r="I17" s="86"/>
-      <c r="J17" s="86"/>
-      <c r="K17" s="86"/>
-      <c r="L17" s="86"/>
-      <c r="M17" s="86" t="s">
+      <c r="I17" s="88"/>
+      <c r="J17" s="88"/>
+      <c r="K17" s="88"/>
+      <c r="L17" s="88"/>
+      <c r="M17" s="88" t="s">
         <v>102</v>
       </c>
-      <c r="N17" s="86"/>
-      <c r="O17" s="86"/>
-      <c r="P17" s="86"/>
+      <c r="N17" s="88"/>
+      <c r="O17" s="88"/>
+      <c r="P17" s="88"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="88" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="89" t="s">
+      <c r="B18" s="90" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="91" t="s">
         <v>103</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="F18" s="90" t="s">
+      <c r="F18" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="G18" s="91" t="s">
+      <c r="G18" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="H18" s="89" t="s">
+      <c r="H18" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="I18" s="89"/>
-      <c r="J18" s="17" t="s">
+      <c r="I18" s="91"/>
+      <c r="J18" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="K18" s="17" t="s">
+      <c r="K18" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="L18" s="90" t="s">
+      <c r="L18" s="92" t="s">
         <v>105</v>
       </c>
-      <c r="M18" s="92" t="s">
+      <c r="M18" s="94" t="s">
         <v>108</v>
       </c>
-      <c r="N18" s="17" t="s">
+      <c r="N18" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="O18" s="17" t="s">
+      <c r="O18" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="P18" s="90" t="s">
+      <c r="P18" s="92" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="88"/>
-      <c r="C19" s="89"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="90"/>
-      <c r="G19" s="91"/>
-      <c r="H19" s="89"/>
-      <c r="I19" s="89"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="90"/>
-      <c r="M19" s="92"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="90"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="91"/>
+      <c r="I19" s="91"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="92"/>
+      <c r="M19" s="94"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="92"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="93" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="94" t="n">
+      <c r="B20" s="95" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="96" t="n">
+        <v>8</v>
+      </c>
+      <c r="D20" s="97" t="n">
         <v>4</v>
       </c>
-      <c r="D20" s="95" t="n">
-        <v>2</v>
-      </c>
-      <c r="E20" s="95" t="n">
-        <v>2</v>
-      </c>
-      <c r="F20" s="96" t="s">
+      <c r="E20" s="97" t="n">
+        <v>4</v>
+      </c>
+      <c r="F20" s="98" t="s">
         <v>109</v>
       </c>
-      <c r="G20" s="97" t="s">
+      <c r="G20" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="H20" s="98" t="s">
+      <c r="H20" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="I20" s="98"/>
-      <c r="J20" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="K20" s="95" t="n">
-        <v>2</v>
-      </c>
-      <c r="L20" s="96" t="n">
+      <c r="I20" s="100"/>
+      <c r="J20" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K20" s="97" t="n">
+        <v>4</v>
+      </c>
+      <c r="L20" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="M20" s="99" t="s">
+      <c r="M20" s="101" t="s">
         <v>70</v>
       </c>
-      <c r="N20" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="O20" s="95" t="n">
-        <v>2</v>
-      </c>
-      <c r="P20" s="96" t="n">
+      <c r="N20" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="O20" s="97" t="n">
+        <v>4</v>
+      </c>
+      <c r="P20" s="98" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M21" s="33"/>
+      <c r="M21" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="36">

</xml_diff>